<commit_message>
revised according to inspection plan C780_PT15_FW_Code_Inspection_Plan_Binary_model.xlsx
</commit_message>
<xml_diff>
--- a/Test/Code_Inspection_Plan_Results/C780_PT15_FW_Code_Inspection_Plan_Binary_model.xlsx
+++ b/Test/Code_Inspection_Plan_Results/C780_PT15_FW_Code_Inspection_Plan_Binary_model.xlsx
@@ -5,23 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hwfwdept_proj\c780_carel_cloud_engine_binary\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hwfwdept_proj\c780_carel_cloud_engine_binary\Test\Code_Inspection_Plan_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="396" yWindow="600" windowWidth="19824" windowHeight="7200" activeTab="2"/>
+    <workbookView xWindow="396" yWindow="600" windowWidth="19824" windowHeight="7200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
-    <sheet name="Files_Check_List" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="115">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -375,259 +374,23 @@
     <t xml:space="preserve">Is there commented out code (for testing) that should be removed? </t>
   </si>
   <si>
-    <t>binary_model.c</t>
+    <t>A.Bilato</t>
   </si>
   <si>
-    <t>binary_model.h</t>
+    <t>OK</t>
   </si>
   <si>
-    <t>CAREL_GLOBAL_DEF.h</t>
+    <t>NA</t>
   </si>
   <si>
-    <t>CBOR_CAREL.c</t>
-  </si>
-  <si>
-    <t>CBOR_CAREL.h</t>
-  </si>
-  <si>
-    <t>CMakeLists.txt</t>
-  </si>
-  <si>
-    <t>common.h</t>
-  </si>
-  <si>
-    <t>component.mk</t>
-  </si>
-  <si>
-    <t>data_types_CAREL.h</t>
-  </si>
-  <si>
-    <t>data_types_IS.h</t>
-  </si>
-  <si>
-    <t>File_System_CAREL.c</t>
-  </si>
-  <si>
-    <t>File_System_CAREL.h</t>
-  </si>
-  <si>
-    <t>File_System_IS.c</t>
-  </si>
-  <si>
-    <t>File_System_IS.h</t>
-  </si>
-  <si>
-    <t>gme_config.h</t>
-  </si>
-  <si>
-    <t>gme_types.h</t>
-  </si>
-  <si>
-    <t>GSM_Miscellaneous_IS.c</t>
-  </si>
-  <si>
-    <t>GSM_Miscellaneous_IS.h</t>
-  </si>
-  <si>
-    <t>https_client_CAREL.c</t>
-  </si>
-  <si>
-    <t>https_client_CAREL.h</t>
-  </si>
-  <si>
-    <t>https_client_IS.c</t>
-  </si>
-  <si>
-    <t>https_client_IS.h</t>
-  </si>
-  <si>
-    <t>http_server_CAREL.c</t>
-  </si>
-  <si>
-    <t>http_server_CAREL.h</t>
-  </si>
-  <si>
-    <t>http_server_IS.c</t>
-  </si>
-  <si>
-    <t>http_server_IS.h</t>
-  </si>
-  <si>
-    <t>IO_Port_IS.c</t>
-  </si>
-  <si>
-    <t>IO_Port_IS.h</t>
-  </si>
-  <si>
-    <t>Kconfig.projbuild</t>
-  </si>
-  <si>
-    <t>Led_Manager_IS.c</t>
-  </si>
-  <si>
-    <t>Led_Manager_IS.h</t>
-  </si>
-  <si>
-    <t>lista.txt</t>
-  </si>
-  <si>
-    <t>main_CAREL.c</t>
-  </si>
-  <si>
-    <t>main_CAREL.h</t>
-  </si>
-  <si>
-    <t>main_IS.c</t>
-  </si>
-  <si>
-    <t>main_IS.h</t>
-  </si>
-  <si>
-    <t>Miscellaneous_IS.h</t>
-  </si>
-  <si>
-    <t>mobile.c</t>
-  </si>
-  <si>
-    <t>mobile.h</t>
-  </si>
-  <si>
-    <t>modbus_IS.c</t>
-  </si>
-  <si>
-    <t>modbus_IS.h</t>
-  </si>
-  <si>
-    <t>MQTT_Interface_CAREL.c</t>
-  </si>
-  <si>
-    <t>MQTT_Interface_CAREL.h</t>
-  </si>
-  <si>
-    <t>MQTT_Interface_IS.c</t>
-  </si>
-  <si>
-    <t>MQTT_Interface_IS.h</t>
-  </si>
-  <si>
-    <t>nvm_CAREL.c</t>
-  </si>
-  <si>
-    <t>nvm_CAREL.h</t>
-  </si>
-  <si>
-    <t>nvm_IS.c</t>
-  </si>
-  <si>
-    <t>nvm_IS.h</t>
-  </si>
-  <si>
-    <t>ota_CAREL.c</t>
-  </si>
-  <si>
-    <t>ota_CAREL.h</t>
-  </si>
-  <si>
-    <t>ota_IS.c</t>
-  </si>
-  <si>
-    <t>ota_IS.h</t>
-  </si>
-  <si>
-    <t>polling_CAREL.c</t>
-  </si>
-  <si>
-    <t>polling_CAREL.h</t>
-  </si>
-  <si>
-    <t>polling_IS.c</t>
-  </si>
-  <si>
-    <t>polling_IS.h</t>
-  </si>
-  <si>
-    <t>radio.c</t>
-  </si>
-  <si>
-    <t>radio.h</t>
-  </si>
-  <si>
-    <t>RTC_IS.c</t>
-  </si>
-  <si>
-    <t>RTC_IS.h</t>
-  </si>
-  <si>
-    <t>SoftWDT.c</t>
-  </si>
-  <si>
-    <t>SoftWDT.h</t>
-  </si>
-  <si>
-    <t>sys_CAREL.c</t>
-  </si>
-  <si>
-    <t>sys_CAREL.h</t>
-  </si>
-  <si>
-    <t>sys_IS.c</t>
-  </si>
-  <si>
-    <t>sys_IS.h</t>
-  </si>
-  <si>
-    <t>test_hw_CAREL.c</t>
-  </si>
-  <si>
-    <t>test_hw_CAREL.h</t>
-  </si>
-  <si>
-    <t>tinycbor</t>
-  </si>
-  <si>
-    <t>types.h</t>
-  </si>
-  <si>
-    <t>utilities_CAREL.c</t>
-  </si>
-  <si>
-    <t>utilities_CAREL.h</t>
-  </si>
-  <si>
-    <t>wifi.c</t>
-  </si>
-  <si>
-    <t>wifi.h</t>
-  </si>
-  <si>
-    <t>File name</t>
-  </si>
-  <si>
-    <t>Revided 
-Assigned to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Link to Excel revision 
-file </t>
-  </si>
-  <si>
-    <t>No.</t>
-  </si>
-  <si>
-    <t>Chiebao</t>
-  </si>
-  <si>
-    <t>Bilato</t>
-  </si>
-  <si>
-    <t>Cellini</t>
+    <t>indirectly by the caller</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -656,12 +419,6 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="SimSun"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1015,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1074,9 +831,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6526,8 +6282,8 @@
   </sheetPr>
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -6603,8 +6359,12 @@
         <v>1</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
+      <c r="D6" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="18">
+        <v>44014</v>
+      </c>
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="13.65" customHeight="1">
@@ -6617,7 +6377,9 @@
       <c r="C7" s="12"/>
       <c r="D7" s="17"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="13.65" customHeight="1">
       <c r="A8" s="34">
@@ -6630,7 +6392,9 @@
       <c r="C8" s="12"/>
       <c r="D8" s="17"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
+      <c r="F8" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="13.65" customHeight="1">
       <c r="A9" s="34">
@@ -6643,7 +6407,9 @@
       <c r="C9" s="12"/>
       <c r="D9" s="17"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
+      <c r="F9" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="13.65" customHeight="1">
       <c r="A10" s="34">
@@ -6656,7 +6422,9 @@
       <c r="C10" s="12"/>
       <c r="D10" s="17"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
+      <c r="F10" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="13.65" customHeight="1">
       <c r="A11" s="34">
@@ -6669,7 +6437,9 @@
       <c r="C11" s="25"/>
       <c r="D11" s="17"/>
       <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
+      <c r="F11" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="13.65" customHeight="1">
       <c r="A12" s="34">
@@ -6682,7 +6452,9 @@
       <c r="C12" s="12"/>
       <c r="D12" s="17"/>
       <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
+      <c r="F12" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="13.65" customHeight="1">
       <c r="A13" s="34">
@@ -6695,7 +6467,9 @@
       <c r="C13" s="12"/>
       <c r="D13" s="17"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
+      <c r="F13" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="13.65" customHeight="1">
       <c r="A14" s="34">
@@ -6708,7 +6482,9 @@
       <c r="C14" s="12"/>
       <c r="D14" s="17"/>
       <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="F14" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="13.65" customHeight="1">
       <c r="A15" s="34"/>
@@ -6730,7 +6506,9 @@
       <c r="C16" s="12"/>
       <c r="D16" s="17"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
+      <c r="F16" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="13.65" customHeight="1">
       <c r="A17" s="34">
@@ -6743,7 +6521,9 @@
       <c r="C17" s="12"/>
       <c r="D17" s="17"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
+      <c r="F17" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="13.65" customHeight="1">
       <c r="A18" s="34">
@@ -6756,7 +6536,9 @@
       <c r="C18" s="12"/>
       <c r="D18" s="17"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
+      <c r="F18" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="13.65" customHeight="1">
       <c r="A19" s="34">
@@ -6769,7 +6551,9 @@
       <c r="C19" s="12"/>
       <c r="D19" s="17"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
+      <c r="F19" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="13.65" customHeight="1">
       <c r="A20" s="34">
@@ -6782,7 +6566,9 @@
       <c r="C20" s="12"/>
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
+      <c r="F20" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="13.65" customHeight="1">
       <c r="A21" s="34">
@@ -6795,7 +6581,9 @@
       <c r="C21" s="12"/>
       <c r="D21" s="17"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="19"/>
+      <c r="F21" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="13.65" customHeight="1">
       <c r="A22" s="34">
@@ -6808,7 +6596,9 @@
       <c r="C22" s="12"/>
       <c r="D22" s="17"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
+      <c r="F22" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="13.65" customHeight="1">
       <c r="A23" s="34">
@@ -6821,7 +6611,9 @@
       <c r="C23" s="12"/>
       <c r="D23" s="17"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="19"/>
+      <c r="F23" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="13.65" customHeight="1">
       <c r="A24" s="34">
@@ -6834,7 +6626,9 @@
       <c r="C24" s="12"/>
       <c r="D24" s="17"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="19"/>
+      <c r="F24" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="13.65" customHeight="1">
       <c r="A25" s="34"/>
@@ -6856,7 +6650,9 @@
       <c r="C26" s="12"/>
       <c r="D26" s="17"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="19"/>
+      <c r="F26" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="13.65" customHeight="1">
       <c r="A27" s="34">
@@ -6869,7 +6665,9 @@
       <c r="C27" s="12"/>
       <c r="D27" s="17"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="19"/>
+      <c r="F27" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="13.65" customHeight="1">
       <c r="A28" s="34">
@@ -6882,7 +6680,9 @@
       <c r="C28" s="12"/>
       <c r="D28" s="17"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="19"/>
+      <c r="F28" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="14.4">
       <c r="A29" s="34">
@@ -6895,7 +6695,9 @@
       <c r="C29" s="12"/>
       <c r="D29" s="17"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="19"/>
+      <c r="F29" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="28.8">
       <c r="A30" s="34">
@@ -6908,7 +6710,9 @@
       <c r="C30" s="12"/>
       <c r="D30" s="17"/>
       <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
+      <c r="F30" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="28.8">
       <c r="A31" s="34">
@@ -6921,7 +6725,9 @@
       <c r="C31" s="12"/>
       <c r="D31" s="17"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="19"/>
+      <c r="F31" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="14.4">
       <c r="A32" s="34">
@@ -6934,7 +6740,9 @@
       <c r="C32" s="12"/>
       <c r="D32" s="17"/>
       <c r="E32" s="18"/>
-      <c r="F32" s="19"/>
+      <c r="F32" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="13.65" customHeight="1">
       <c r="A33" s="34"/>
@@ -6956,7 +6764,9 @@
       <c r="C34" s="12"/>
       <c r="D34" s="17"/>
       <c r="E34" s="18"/>
-      <c r="F34" s="19"/>
+      <c r="F34" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="13.65" customHeight="1">
       <c r="A35" s="34">
@@ -6969,7 +6779,9 @@
       <c r="C35" s="20"/>
       <c r="D35" s="17"/>
       <c r="E35" s="18"/>
-      <c r="F35" s="19"/>
+      <c r="F35" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="13.65" customHeight="1">
       <c r="A36" s="34">
@@ -6982,7 +6794,9 @@
       <c r="C36" s="20"/>
       <c r="D36" s="17"/>
       <c r="E36" s="18"/>
-      <c r="F36" s="19"/>
+      <c r="F36" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="13.65" customHeight="1">
       <c r="A37" s="34">
@@ -6995,7 +6809,9 @@
       <c r="C37" s="12"/>
       <c r="D37" s="17"/>
       <c r="E37" s="18"/>
-      <c r="F37" s="19"/>
+      <c r="F37" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="13.65" customHeight="1">
       <c r="A38" s="34">
@@ -7008,7 +6824,9 @@
       <c r="C38" s="12"/>
       <c r="D38" s="17"/>
       <c r="E38" s="18"/>
-      <c r="F38" s="19"/>
+      <c r="F38" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="13.65" customHeight="1">
       <c r="A39" s="34">
@@ -7021,7 +6839,9 @@
       <c r="C39" s="12"/>
       <c r="D39" s="17"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="19"/>
+      <c r="F39" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="13.65" customHeight="1">
       <c r="A40" s="34">
@@ -7034,7 +6854,9 @@
       <c r="C40" s="20"/>
       <c r="D40" s="17"/>
       <c r="E40" s="18"/>
-      <c r="F40" s="19"/>
+      <c r="F40" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="13.65" customHeight="1">
       <c r="A41" s="34">
@@ -7047,7 +6869,9 @@
       <c r="C41" s="20"/>
       <c r="D41" s="17"/>
       <c r="E41" s="18"/>
-      <c r="F41" s="19"/>
+      <c r="F41" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="13.65" customHeight="1">
       <c r="A42" s="34"/>
@@ -7069,7 +6893,9 @@
       <c r="C43" s="12"/>
       <c r="D43" s="17"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="19"/>
+      <c r="F43" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="13.65" customHeight="1">
       <c r="A44" s="34">
@@ -7082,7 +6908,9 @@
       <c r="C44" s="12"/>
       <c r="D44" s="17"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="19"/>
+      <c r="F44" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="13.65" customHeight="1">
       <c r="A45" s="34">
@@ -7095,7 +6923,9 @@
       <c r="C45" s="12"/>
       <c r="D45" s="17"/>
       <c r="E45" s="18"/>
-      <c r="F45" s="19"/>
+      <c r="F45" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="13.65" customHeight="1">
       <c r="A46" s="34">
@@ -7108,7 +6938,9 @@
       <c r="C46" s="12"/>
       <c r="D46" s="17"/>
       <c r="E46" s="18"/>
-      <c r="F46" s="19"/>
+      <c r="F46" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="13.65" customHeight="1">
       <c r="A47" s="34">
@@ -7121,7 +6953,9 @@
       <c r="C47" s="12"/>
       <c r="D47" s="17"/>
       <c r="E47" s="18"/>
-      <c r="F47" s="19"/>
+      <c r="F47" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="13.65" customHeight="1">
       <c r="A48" s="34">
@@ -7134,7 +6968,9 @@
       <c r="C48" s="12"/>
       <c r="D48" s="17"/>
       <c r="E48" s="18"/>
-      <c r="F48" s="19"/>
+      <c r="F48" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="13.65" customHeight="1">
       <c r="A49" s="34"/>
@@ -7156,7 +6992,9 @@
       <c r="C50" s="12"/>
       <c r="D50" s="17"/>
       <c r="E50" s="18"/>
-      <c r="F50" s="19"/>
+      <c r="F50" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="13.65" customHeight="1">
       <c r="A51" s="34">
@@ -7169,7 +7007,9 @@
       <c r="C51" s="12"/>
       <c r="D51" s="17"/>
       <c r="E51" s="18"/>
-      <c r="F51" s="19"/>
+      <c r="F51" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="13.65" customHeight="1">
       <c r="A52" s="34">
@@ -7182,7 +7022,9 @@
       <c r="C52" s="12"/>
       <c r="D52" s="17"/>
       <c r="E52" s="18"/>
-      <c r="F52" s="19"/>
+      <c r="F52" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="13.65" customHeight="1">
       <c r="A53" s="34">
@@ -7195,7 +7037,9 @@
       <c r="C53" s="12"/>
       <c r="D53" s="17"/>
       <c r="E53" s="18"/>
-      <c r="F53" s="19"/>
+      <c r="F53" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="13.65" customHeight="1">
       <c r="A54" s="34">
@@ -7205,10 +7049,14 @@
       <c r="B54" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="12"/>
+      <c r="C54" s="20" t="s">
+        <v>114</v>
+      </c>
       <c r="D54" s="17"/>
       <c r="E54" s="18"/>
-      <c r="F54" s="19"/>
+      <c r="F54" s="40" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="13.65" customHeight="1">
       <c r="A55" s="34">
@@ -7231,10 +7079,14 @@
       <c r="B56" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="12"/>
+      <c r="C56" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="D56" s="17"/>
       <c r="E56" s="18"/>
-      <c r="F56" s="19"/>
+      <c r="F56" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="13.65" customHeight="1">
       <c r="A57" s="34">
@@ -7247,7 +7099,9 @@
       <c r="C57" s="20"/>
       <c r="D57" s="17"/>
       <c r="E57" s="18"/>
-      <c r="F57" s="19"/>
+      <c r="F57" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="13.65" customHeight="1">
       <c r="A58" s="34">
@@ -7260,7 +7114,9 @@
       <c r="C58" s="12"/>
       <c r="D58" s="17"/>
       <c r="E58" s="18"/>
-      <c r="F58" s="19"/>
+      <c r="F58" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="13.65" customHeight="1">
       <c r="A59" s="34"/>
@@ -14790,866 +14646,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D76"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="43.2">
-      <c r="A1" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>135</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>136</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>138</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>142</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>143</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>144</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>146</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>148</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>151</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>152</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>154</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>157</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>159</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>160</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>161</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>162</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>163</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="1">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>164</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>165</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="1">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>166</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>167</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>168</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1">
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>170</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="1">
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>171</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="1">
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>172</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>173</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>174</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>175</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>176</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>177</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1">
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>178</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1">
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
-        <v>179</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>180</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1">
-        <v>71</v>
-      </c>
-      <c r="B72" t="s">
-        <v>181</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1">
-        <v>72</v>
-      </c>
-      <c r="B73" t="s">
-        <v>182</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1">
-        <v>73</v>
-      </c>
-      <c r="B74" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1">
-        <v>74</v>
-      </c>
-      <c r="B75" t="s">
-        <v>184</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="1">
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>185</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>